<commit_message>
Modified VCEA_goals to fit naming conventions. Created metadata file for VCEA_goals.
</commit_message>
<xml_diff>
--- a/data/VCEA_goals.xlsx
+++ b/data/VCEA_goals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyung\Documents\GitHub\postgres-etl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD58252B-AE2B-4ED4-BA14-217B7472EB5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388F152D-B7CC-411D-844B-1F980B5659A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2868" yWindow="2868" windowWidth="8640" windowHeight="4224" xr2:uid="{2BE932FA-E61C-4F47-B3CF-1F177F70D416}"/>
+    <workbookView xWindow="18240" yWindow="2700" windowWidth="8640" windowHeight="4224" xr2:uid="{2BE932FA-E61C-4F47-B3CF-1F177F70D416}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,22 @@
     <t>dominion_energy_efficiency_as_share_of_2019_sales</t>
   </si>
   <si>
-    <t>apco_onshore_wind_and_solar_(Megawatts)</t>
+    <t>apco_onshore_wind_and_solar_MW</t>
   </si>
   <si>
-    <t>dominion_onshore_wind_and_solar_(Megawatts)</t>
+    <t>dominion_onshore_wind_and_solar_MW</t>
   </si>
   <si>
-    <t>apco_storage_(Megawatts)</t>
+    <t>apco_storage_MW</t>
   </si>
   <si>
-    <t>dominion_storage_(Megawatts)</t>
+    <t>dominion_storage_MW</t>
   </si>
   <si>
-    <t>apco_rps (%)</t>
+    <t>apco_rps</t>
   </si>
   <si>
-    <t>dominion_rps (%)</t>
+    <t xml:space="preserve">dominion_rps </t>
   </si>
 </sst>
 </file>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2204A34C-DF71-FD48-B1BE-2A1EE1E43562}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>

</xml_diff>

<commit_message>
Modified syntax and wording of fields.
</commit_message>
<xml_diff>
--- a/data/VCEA_goals.xlsx
+++ b/data/VCEA_goals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyung\Documents\GitHub\postgres-etl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388F152D-B7CC-411D-844B-1F980B5659A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42E2FCA-CC74-47A2-BC9C-9E87180B38AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18240" yWindow="2700" windowWidth="8640" windowHeight="4224" xr2:uid="{2BE932FA-E61C-4F47-B3CF-1F177F70D416}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2BE932FA-E61C-4F47-B3CF-1F177F70D416}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,22 +36,22 @@
     <t>dominion_energy_efficiency_as_share_of_2019_sales</t>
   </si>
   <si>
-    <t>apco_onshore_wind_and_solar_MW</t>
-  </si>
-  <si>
-    <t>dominion_onshore_wind_and_solar_MW</t>
-  </si>
-  <si>
-    <t>apco_storage_MW</t>
-  </si>
-  <si>
-    <t>dominion_storage_MW</t>
-  </si>
-  <si>
     <t>apco_rps</t>
   </si>
   <si>
     <t xml:space="preserve">dominion_rps </t>
+  </si>
+  <si>
+    <t>apco_onshore_wind_and_solar_mw</t>
+  </si>
+  <si>
+    <t>dominion_onshore_wind_and_solar_mw</t>
+  </si>
+  <si>
+    <t>apco_storage_mw</t>
+  </si>
+  <si>
+    <t>dominion_storage_mw</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -430,22 +430,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Updated the quantitative goals to be cumulitative.
</commit_message>
<xml_diff>
--- a/data/VCEA_goals.xlsx
+++ b/data/VCEA_goals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pyung\Documents\GitHub\postgres-etl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42E2FCA-CC74-47A2-BC9C-9E87180B38AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDF5F7E-1CA1-4332-8F70-5E23621AC6FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2BE932FA-E61C-4F47-B3CF-1F177F70D416}"/>
   </bookViews>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2204A34C-DF71-FD48-B1BE-2A1EE1E43562}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -587,10 +587,10 @@
         <v>0.32</v>
       </c>
       <c r="D8" s="1">
-        <v>200</v>
+        <v>400</v>
       </c>
       <c r="E8" s="1">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -642,10 +642,10 @@
         <v>0.41</v>
       </c>
       <c r="D11" s="1">
-        <v>200</v>
+        <v>600</v>
       </c>
       <c r="E11" s="1">
-        <v>4000</v>
+        <v>10000</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -732,7 +732,7 @@
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1">
-        <v>6100</v>
+        <v>16100</v>
       </c>
       <c r="F16" s="1">
         <v>400</v>

</xml_diff>